<commit_message>
Add integration tests for inventory management and update database schema
- Implemented a new test case to handle insufficient stock reservations in `test_inventario_integracion.py`.
- Enhanced existing tests to verify item attributes and stock management.
- Created a unified SQL script for critical table structures in the MPS system, including `inventario_perfiles`, `usuarios`, and others.
- Added PDF files for audit and inventory documentation.
</commit_message>
<xml_diff>
--- a/inventario.xlsx
+++ b/inventario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,108 +490,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123456.789</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Material A</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>PVC</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>unidad</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>100</v>
-      </c>
-      <c r="G2" t="n">
-        <v>10</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Almacén 1</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Descripción A</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>QR123</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>imagen_a.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>987654.321</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Material B</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Aluminio</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>kg</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>50</v>
-      </c>
-      <c r="G3" t="n">
-        <v>5</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Almacén 2</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Descripción B</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>QR987</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>imagen_b.jpg</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>